<commit_message>
Standardise author names among other changes
Delete add theories and move functionality into iniToJson
Have statistics and keywords generated every time
</commit_message>
<xml_diff>
--- a/report/SUS.xlsx
+++ b/report/SUS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carli\Desktop\afp\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{095EEA91-415D-46F2-A177-52309379135C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CDA93A-DFDE-42CF-AF8A-AA121CB44DE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4388" yWindow="3308" windowWidth="16065" windowHeight="10972" xr2:uid="{AC616F52-0775-42A2-8179-B854D5F33AF2}"/>
+    <workbookView xWindow="1670" yWindow="8230" windowWidth="17700" windowHeight="10840" xr2:uid="{AC616F52-0775-42A2-8179-B854D5F33AF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,21 +457,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052E3F4E-A412-4E62-A76B-5A42D090A9EB}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.86328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="52.81640625" style="4" customWidth="1"/>
     <col min="2" max="7" width="4" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" style="4"/>
+    <col min="8" max="8" width="9.08984375" style="4"/>
     <col min="9" max="14" width="6" style="4" customWidth="1"/>
-    <col min="15" max="15" width="8.265625" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.06640625" style="4"/>
+    <col min="15" max="15" width="8.26953125" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -518,7 +518,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,31 +541,31 @@
         <v>1</v>
       </c>
       <c r="I3" s="4">
-        <f>B3-1</f>
+        <f t="shared" ref="I3:N3" si="0">B3-1</f>
         <v>-1</v>
       </c>
       <c r="J3" s="4">
-        <f>C3-1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K3" s="4">
-        <f>D3-1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L3" s="4">
-        <f>E3-1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M3" s="4">
-        <f>F3-1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N3" s="4">
-        <f>G3-1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -592,27 +592,27 @@
         <v>4</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:N4" si="0">5-C4</f>
+        <f t="shared" ref="J4:N4" si="1">5-C4</f>
         <v>2</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -639,19 +639,19 @@
         <v>0</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5" si="1">C5-1</f>
+        <f t="shared" ref="J5" si="2">C5-1</f>
         <v>0</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" ref="K5" si="2">D5-1</f>
+        <f t="shared" ref="K5" si="3">D5-1</f>
         <v>2</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" ref="L5" si="3">E5-1</f>
+        <f t="shared" ref="L5" si="4">E5-1</f>
         <v>1</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5" si="4">F5-1</f>
+        <f t="shared" ref="M5" si="5">F5-1</f>
         <v>2</v>
       </c>
       <c r="N5" s="4">
@@ -659,7 +659,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -686,27 +686,27 @@
         <v>5</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" ref="J6" si="5">5-C6</f>
+        <f t="shared" ref="J6" si="6">5-C6</f>
         <v>4</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" ref="K6" si="6">5-D6</f>
+        <f t="shared" ref="K6" si="7">5-D6</f>
         <v>3</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" ref="L6" si="7">5-E6</f>
+        <f t="shared" ref="L6" si="8">5-E6</f>
         <v>3</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6" si="8">5-F6</f>
+        <f t="shared" ref="M6" si="9">5-F6</f>
         <v>5</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6" si="9">5-G6</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="30.75" x14ac:dyDescent="0.45">
+        <f t="shared" ref="N6" si="10">5-G6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -733,19 +733,19 @@
         <v>1</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" ref="J7" si="10">C7-1</f>
+        <f t="shared" ref="J7" si="11">C7-1</f>
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" ref="K7" si="11">D7-1</f>
+        <f t="shared" ref="K7" si="12">D7-1</f>
         <v>1</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7" si="12">E7-1</f>
+        <f t="shared" ref="L7" si="13">E7-1</f>
         <v>0</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" ref="M7" si="13">F7-1</f>
+        <f t="shared" ref="M7" si="14">F7-1</f>
         <v>0</v>
       </c>
       <c r="N7" s="4">
@@ -753,7 +753,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -780,27 +780,27 @@
         <v>3</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" ref="J8" si="14">5-C8</f>
+        <f t="shared" ref="J8" si="15">5-C8</f>
         <v>3</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" ref="K8" si="15">5-D8</f>
+        <f t="shared" ref="K8" si="16">5-D8</f>
         <v>3</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" ref="L8" si="16">5-E8</f>
+        <f t="shared" ref="L8" si="17">5-E8</f>
         <v>3</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" ref="M8" si="17">5-F8</f>
+        <f t="shared" ref="M8" si="18">5-F8</f>
         <v>4</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" ref="N8" si="18">5-G8</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30.75" x14ac:dyDescent="0.45">
+        <f t="shared" ref="N8" si="19">5-G8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -827,19 +827,19 @@
         <v>2</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" ref="J9" si="19">C9-1</f>
+        <f t="shared" ref="J9" si="20">C9-1</f>
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" ref="K9" si="20">D9-1</f>
+        <f t="shared" ref="K9" si="21">D9-1</f>
         <v>2</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" ref="L9" si="21">E9-1</f>
+        <f t="shared" ref="L9" si="22">E9-1</f>
         <v>1</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" ref="M9" si="22">F9-1</f>
+        <f t="shared" ref="M9" si="23">F9-1</f>
         <v>1</v>
       </c>
       <c r="N9" s="4">
@@ -847,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -874,27 +874,27 @@
         <v>2</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" ref="J10" si="23">5-C10</f>
+        <f t="shared" ref="J10" si="24">5-C10</f>
         <v>2</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" ref="K10" si="24">5-D10</f>
+        <f t="shared" ref="K10" si="25">5-D10</f>
         <v>4</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ref="L10" si="25">5-E10</f>
+        <f t="shared" ref="L10" si="26">5-E10</f>
         <v>2</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" ref="M10" si="26">5-F10</f>
+        <f t="shared" ref="M10" si="27">5-F10</f>
         <v>5</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" ref="N10" si="27">5-G10</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+        <f t="shared" ref="N10" si="28">5-G10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -921,19 +921,19 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" ref="J11" si="28">C11-1</f>
+        <f t="shared" ref="J11" si="29">C11-1</f>
         <v>1</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" ref="K11" si="29">D11-1</f>
+        <f t="shared" ref="K11" si="30">D11-1</f>
         <v>2</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ref="L11" si="30">E11-1</f>
+        <f t="shared" ref="L11" si="31">E11-1</f>
         <v>0</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" ref="M11" si="31">F11-1</f>
+        <f t="shared" ref="M11" si="32">F11-1</f>
         <v>2</v>
       </c>
       <c r="N11" s="4">
@@ -941,81 +941,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
+      <c r="B12" s="1">
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>2</v>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
       </c>
       <c r="I12" s="4">
         <f>5-B12</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" ref="J12" si="32">5-C12</f>
-        <v>3</v>
+        <f t="shared" ref="J12" si="33">5-C12</f>
+        <v>2</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" ref="K12" si="33">5-D12</f>
-        <v>4</v>
+        <f t="shared" ref="K12" si="34">5-D12</f>
+        <v>2</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12" si="34">5-E12</f>
+        <f t="shared" ref="L12" si="35">5-E12</f>
         <v>2</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" ref="M12" si="35">5-F12</f>
-        <v>4</v>
+        <f t="shared" ref="M12" si="36">5-F12</f>
+        <v>2</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" ref="N12" si="36">5-G12</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+        <f t="shared" ref="N12" si="37">5-G12</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I13" s="4">
         <f>SUM(I3:I12)*2.5</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" ref="J13:N13" si="37">SUM(J3:J12)*2.5</f>
-        <v>42.5</v>
+        <f t="shared" ref="J13:N13" si="38">SUM(J3:J12)*2.5</f>
+        <v>40</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="37"/>
-        <v>67.5</v>
+        <f t="shared" si="38"/>
+        <v>62.5</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>35</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="37"/>
-        <v>67.5</v>
+        <f t="shared" si="38"/>
+        <v>62.5</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="37"/>
-        <v>32.5</v>
+        <f t="shared" si="38"/>
+        <v>30</v>
       </c>
       <c r="O13" s="4">
         <f>AVERAGE(I13:N13)</f>
-        <v>49.166666666666664</v>
+        <v>45.833333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>